<commit_message>
#148 optional run var prefix for EachCommand.groupBy and .orderBy
- catch NullPointerException for better error display
- added prefix "d." for groupBy in an Excel template file
- added prefix for orderBy attribute in OrderByTest.xlsx
- removeVarPrefix() not necessary for groupBy
</commit_message>
<xml_diff>
--- a/jxls-poi/src/test/resources/org/jxls/templatebasedtests/GroupSumTest_filterCondition.xlsx
+++ b/jxls-poi/src/test/resources/org/jxls/templatebasedtests/GroupSumTest_filterCondition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\JobStuff\GitRepos\jxls\jxls-poi\src\test\resources\org\jxls\templatebasedtests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CB6C4E-1828-4FC8-B050-BE805530EC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4310AFA3-09AF-4DF5-81BE-D5BC7513EB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
           </rPr>
           <t xml:space="preserve">
 // departments:
-jx:each(items="details", var="d", groupBy="buGroup", groupOrder="asc", lastCell="F7")</t>
+jx:each(items="details", var="d", groupBy="d.buGroup", groupOrder="asc", lastCell="F7")</t>
         </r>
       </text>
     </comment>

</xml_diff>